<commit_message>
some progress in purchas/sale conversion
</commit_message>
<xml_diff>
--- a/samples/sample_FT_error.xlsx
+++ b/samples/sample_FT_error.xlsx
@@ -315,7 +315,7 @@
     <t>01609W102</t>
   </si>
   <si>
-    <t>G1: settle day too early</t>
+    <t>G14: settle day too early</t>
   </si>
 </sst>
 </file>
@@ -1134,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,8 +1266,8 @@
       <c r="F2">
         <v>8042016</v>
       </c>
-      <c r="G2" s="4">
-        <v>8032016</v>
+      <c r="G2">
+        <v>8042016</v>
       </c>
       <c r="H2">
         <v>8042016</v>
@@ -2016,8 +2016,8 @@
       <c r="F14">
         <v>6142016</v>
       </c>
-      <c r="G14">
-        <v>6162016</v>
+      <c r="G14" s="4">
+        <v>6122016</v>
       </c>
       <c r="H14">
         <v>6142016</v>
@@ -2105,8 +2105,8 @@
       <c r="J15">
         <v>-5211150</v>
       </c>
-      <c r="K15">
-        <v>-5211150</v>
+      <c r="K15" s="4">
+        <v>-5211149</v>
       </c>
       <c r="L15">
         <v>0</v>

</xml_diff>